<commit_message>
Cleaned up Excel files for 2016 CONCACAF Olympic Qualifiers
</commit_message>
<xml_diff>
--- a/source/excel/2016-olympic-qualifiers-concacaf/2016-olympic-qualifiers-concacaf-usa-can-022116.xlsx
+++ b/source/excel/2016-olympic-qualifiers-concacaf/2016-olympic-qualifiers-concacaf-usa-can-022116.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Documents/WoSo Stats Testbed/source/excel/2016-olympic-qualifiers-concacaf/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/wosostats/source/excel/2016-olympic-qualifiers-concacaf/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="9800" windowWidth="22220" windowHeight="5860" tabRatio="500"/>
+    <workbookView xWindow="2440" yWindow="1900" windowWidth="22220" windowHeight="11340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="match" sheetId="1" r:id="rId1"/>
@@ -2629,8 +2629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1398"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1294" workbookViewId="0">
-      <selection activeCell="G1300" sqref="G1300"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>